<commit_message>
add all pre files
</commit_message>
<xml_diff>
--- a/任务表.xlsx
+++ b/任务表.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{B05E5325-8A17-4678-AC3A-CDC4EA1255BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD07237C-849B-4258-AD1F-D1E4C6519548}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="易方达消费行业" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="142">
   <si>
     <t>事项</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -424,13 +429,167 @@
   <si>
     <t>d20 同房</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白酒子行业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白色家电板块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G20峰会</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利好</t>
+  </si>
+  <si>
+    <t>股票型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>易方达消费行业股票型证券投资基金</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基金全称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基金代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成立日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基金类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资产规模</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>175.24亿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基金管理人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>易方达基金管理有限公司</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基金托管人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国农业银行股份有限公司</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基金经理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>萧楠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基金名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>易方达消费行业股票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>易方达大健康主题灵活配置混合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>易方达现代服务业灵活配置混合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>易方达瑞恒灵活配置混合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>广州市黄埔区城市管理和综合执法局</t>
+  </si>
+  <si>
+    <t>QD201810190143</t>
+  </si>
+  <si>
+    <t>清洁卫生车辆</t>
+  </si>
+  <si>
+    <t>已上报</t>
+  </si>
+  <si>
+    <t>QD201904230085</t>
+  </si>
+  <si>
+    <t>2019-2021生活垃圾分类智能分类运行服务</t>
+  </si>
+  <si>
+    <t>QD201902030019</t>
+  </si>
+  <si>
+    <t>城镇公共卫生服务</t>
+  </si>
+  <si>
+    <t>QD201902270046</t>
+  </si>
+  <si>
+    <t>长洲岛地埋式生活垃圾直收运项目</t>
+  </si>
+  <si>
+    <t>QD201902270040</t>
+  </si>
+  <si>
+    <t>科学城转动站压缩设备升级改造</t>
+  </si>
+  <si>
+    <t>QD201904170126</t>
+  </si>
+  <si>
+    <t>台式电脑</t>
+  </si>
+  <si>
+    <t>QD201903150090</t>
+  </si>
+  <si>
+    <t>运行维护服务</t>
+  </si>
+  <si>
+    <t>QD201904170130</t>
+  </si>
+  <si>
+    <t>碎纸机</t>
+  </si>
+  <si>
+    <t>编辑</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="182" formatCode="#,##0.000000"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,8 +611,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000033"/>
+      <name val="Inherit"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000033"/>
+      <name val="Inherit"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,8 +658,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFECF5FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -496,11 +694,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF99BBE8"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF99BBE8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF99BBE8"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF99BBE8"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF99BBE8"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF99BBE8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF99BBE8"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF99BBE8"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF99BBE8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF99BBE8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF99BBE8"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF99BBE8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF99BBE8"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF99BBE8"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF99BBE8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF99BBE8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -523,6 +802,62 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -538,6 +873,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>7353</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>180726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C5A1191-FC2D-47EF-949A-DD8CDD79F556}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4124325" y="20059650"/>
+          <a:ext cx="17371428" cy="1990476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>312287</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>123515</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75A8726E-1ADD-45A1-9DF8-664DE7E41E55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4124325" y="22231350"/>
+          <a:ext cx="16304762" cy="2476190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -809,13 +1237,13 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="7.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="32" width="3.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" s="1" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -913,7 +1341,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -949,7 +1377,7 @@
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -985,7 +1413,7 @@
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1021,7 +1449,7 @@
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1057,7 +1485,7 @@
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1093,7 +1521,7 @@
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1129,7 +1557,7 @@
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1165,7 +1593,7 @@
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1201,7 +1629,7 @@
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1237,7 +1665,7 @@
       <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1701,7 @@
       <c r="AE11" s="4"/>
       <c r="AF11" s="4"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1309,7 +1737,7 @@
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1345,7 +1773,7 @@
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1381,7 +1809,7 @@
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1417,7 +1845,7 @@
       <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1453,7 +1881,7 @@
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1489,7 +1917,7 @@
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -1525,7 +1953,7 @@
       <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1561,7 +1989,7 @@
       <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -1597,7 +2025,7 @@
       <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1633,7 +2061,7 @@
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1669,7 +2097,7 @@
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -1705,7 +2133,7 @@
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -1741,7 +2169,7 @@
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -1777,7 +2205,7 @@
       <c r="AE25" s="4"/>
       <c r="AF25" s="4"/>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32">
       <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
@@ -1822,13 +2250,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53322BD8-42F1-42D6-B055-25C9C81B1B2A}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="I124" sqref="I124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.375" bestFit="1" customWidth="1"/>
@@ -1843,7 +2271,7 @@
     <col min="12" max="12" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1884,7 +2312,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="42.75">
       <c r="C2" s="6" t="s">
         <v>36</v>
       </c>
@@ -1904,7 +2332,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>20160127</v>
       </c>
@@ -1918,7 +2346,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>20160706</v>
       </c>
@@ -1932,7 +2360,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>20160902</v>
       </c>
@@ -1946,7 +2374,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>20161114</v>
       </c>
@@ -1960,7 +2388,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>20170208</v>
       </c>
@@ -1974,7 +2402,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>20171123</v>
       </c>
@@ -1988,7 +2416,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>20180818</v>
       </c>
@@ -2002,7 +2430,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>20181121</v>
       </c>
@@ -2025,7 +2453,7 @@
         <v>28.16</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>20181123</v>
       </c>
@@ -2033,7 +2461,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>20181202</v>
       </c>
@@ -2041,7 +2469,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>20181204</v>
       </c>
@@ -2067,7 +2495,7 @@
         <v>22.72</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>20181206</v>
       </c>
@@ -2075,7 +2503,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>20181231</v>
       </c>
@@ -2083,7 +2511,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>20190103</v>
       </c>
@@ -2109,7 +2537,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>20190107</v>
       </c>
@@ -2117,7 +2545,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>20190202</v>
       </c>
@@ -2125,7 +2553,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>20190207</v>
       </c>
@@ -2133,7 +2561,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="8">
         <v>20190306</v>
       </c>
@@ -2141,7 +2569,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="8">
         <v>20190308</v>
       </c>
@@ -2158,7 +2586,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="8">
         <v>20190309</v>
       </c>
@@ -2169,7 +2597,7 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="8">
         <v>20190314</v>
       </c>
@@ -2186,7 +2614,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="8">
         <v>20190318</v>
       </c>
@@ -2212,7 +2640,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="8">
         <v>20190320</v>
       </c>
@@ -2238,7 +2666,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" s="8">
         <v>20190321</v>
       </c>
@@ -2264,7 +2692,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="8">
         <v>20190322</v>
       </c>
@@ -2275,7 +2703,7 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="8">
         <v>20190323</v>
       </c>
@@ -2286,7 +2714,7 @@
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="8">
         <v>20190325</v>
       </c>
@@ -2312,7 +2740,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" s="8">
         <v>20190404</v>
       </c>
@@ -2328,7 +2756,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>20190408</v>
       </c>
@@ -2337,7 +2765,7 @@
       </c>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>20190410</v>
       </c>
@@ -2364,7 +2792,7 @@
       </c>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33">
         <v>20190411</v>
       </c>
@@ -2373,7 +2801,7 @@
       </c>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="9">
         <v>20190507</v>
       </c>
@@ -2382,7 +2810,7 @@
       </c>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="9">
         <v>20190510</v>
       </c>
@@ -2417,7 +2845,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="9">
         <v>20190511</v>
       </c>
@@ -2428,7 +2856,7 @@
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="9">
         <v>20190517</v>
       </c>
@@ -2445,7 +2873,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="9">
         <v>20190520</v>
       </c>
@@ -2471,7 +2899,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="9">
         <v>20190521</v>
       </c>
@@ -2497,7 +2925,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13">
       <c r="A40" s="9">
         <v>20190522</v>
       </c>
@@ -2523,7 +2951,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13">
       <c r="A41" s="9">
         <v>20190523</v>
       </c>
@@ -2549,7 +2977,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" s="9">
         <v>20190524</v>
       </c>
@@ -2560,7 +2988,7 @@
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13">
       <c r="A43" s="9">
         <v>20190525</v>
       </c>
@@ -2571,7 +2999,7 @@
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13">
       <c r="A44" s="9">
         <v>20190526</v>
       </c>
@@ -2582,7 +3010,7 @@
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13">
       <c r="A45" s="9">
         <v>20190527</v>
       </c>
@@ -2611,7 +3039,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13">
       <c r="A46" s="9">
         <v>20190610</v>
       </c>
@@ -2624,6 +3052,291 @@
       </c>
       <c r="L46" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="6:14" ht="15" thickBot="1"/>
+    <row r="74" spans="6:14" ht="15" thickBot="1">
+      <c r="H74" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="I74" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="J74" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="K74" s="29"/>
+      <c r="L74" s="29"/>
+      <c r="M74" s="29"/>
+      <c r="N74" s="30"/>
+    </row>
+    <row r="75" spans="6:14" ht="48.75" thickBot="1">
+      <c r="F75" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G75" s="19">
+        <v>43643</v>
+      </c>
+      <c r="H75" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="I75" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="J75" s="20">
+        <v>1743</v>
+      </c>
+      <c r="K75" s="20">
+        <v>1552.5</v>
+      </c>
+      <c r="L75" s="19">
+        <v>43655</v>
+      </c>
+      <c r="M75" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="N75" s="21">
+        <v>201906</v>
+      </c>
+    </row>
+    <row r="76" spans="6:14" ht="60.75" thickBot="1">
+      <c r="F76" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="G76" s="23">
+        <v>43616</v>
+      </c>
+      <c r="H76" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I76" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="J76" s="24">
+        <v>1890</v>
+      </c>
+      <c r="K76" s="24">
+        <v>1700</v>
+      </c>
+      <c r="L76" s="23">
+        <v>43655</v>
+      </c>
+      <c r="M76" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="N76" s="17">
+        <v>201906</v>
+      </c>
+    </row>
+    <row r="77" spans="6:14" ht="48.75" thickBot="1">
+      <c r="F77" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G77" s="19">
+        <v>43540</v>
+      </c>
+      <c r="H77" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="I77" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="J77" s="20">
+        <v>40062.160000000003</v>
+      </c>
+      <c r="K77" s="20">
+        <v>40062.160000000003</v>
+      </c>
+      <c r="L77" s="19">
+        <v>43655</v>
+      </c>
+      <c r="M77" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="N77" s="21">
+        <v>201906</v>
+      </c>
+    </row>
+    <row r="78" spans="6:14" ht="48.75" thickBot="1">
+      <c r="F78" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="G78" s="23">
+        <v>43607</v>
+      </c>
+      <c r="H78" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="I78" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="J78" s="22">
+        <v>925</v>
+      </c>
+      <c r="K78" s="22">
+        <v>916.98</v>
+      </c>
+      <c r="L78" s="23">
+        <v>43655</v>
+      </c>
+      <c r="M78" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="N78" s="17">
+        <v>201905</v>
+      </c>
+    </row>
+    <row r="79" spans="6:14" ht="48.75" thickBot="1">
+      <c r="F79" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G79" s="19">
+        <v>43607</v>
+      </c>
+      <c r="H79" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="I79" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="J79" s="18">
+        <v>550</v>
+      </c>
+      <c r="K79" s="18">
+        <v>460</v>
+      </c>
+      <c r="L79" s="19">
+        <v>43655</v>
+      </c>
+      <c r="M79" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="N79" s="21">
+        <v>201905</v>
+      </c>
+    </row>
+    <row r="80" spans="6:14" ht="48.75" thickBot="1">
+      <c r="F80" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="G80" s="23">
+        <v>43598</v>
+      </c>
+      <c r="H80" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="I80" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="J80" s="22">
+        <v>12</v>
+      </c>
+      <c r="K80" s="22">
+        <v>11.997999999999999</v>
+      </c>
+      <c r="L80" s="23">
+        <v>43655</v>
+      </c>
+      <c r="M80" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="N80" s="17">
+        <v>201905</v>
+      </c>
+    </row>
+    <row r="81" spans="6:14" ht="48.75" thickBot="1">
+      <c r="F81" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G81" s="19">
+        <v>43553</v>
+      </c>
+      <c r="H81" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="I81" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J81" s="18">
+        <v>117.65</v>
+      </c>
+      <c r="K81" s="18">
+        <v>117.644576</v>
+      </c>
+      <c r="L81" s="19">
+        <v>43655</v>
+      </c>
+      <c r="M81" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="N81" s="21">
+        <v>201904</v>
+      </c>
+    </row>
+    <row r="82" spans="6:14" ht="48.75" thickBot="1">
+      <c r="F82" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="G82" s="23">
+        <v>43598</v>
+      </c>
+      <c r="H82" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="I82" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+      <c r="K82" s="22">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="L82" s="23">
+        <v>43655</v>
+      </c>
+      <c r="M82" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="N82" s="17">
+        <v>201905</v>
+      </c>
+    </row>
+    <row r="83" spans="6:14" ht="48.75" thickBot="1">
+      <c r="F83" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G83" s="19">
+        <v>43598</v>
+      </c>
+      <c r="H83" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I83" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="J83" s="18"/>
+      <c r="K83" s="18"/>
+      <c r="L83" s="16"/>
+      <c r="M83" s="16"/>
+      <c r="N83" s="33"/>
+    </row>
+    <row r="84" spans="6:14" ht="15" thickBot="1">
+      <c r="J84" s="35">
+        <f>SUM(J75:J83)</f>
+        <v>45300.810000000005</v>
+      </c>
+      <c r="K84" s="34">
+        <f>SUM(K75:K83)</f>
+        <v>44822.282076000003</v>
+      </c>
+    </row>
+    <row r="85" spans="6:14" ht="15" thickBot="1">
+      <c r="J85" s="25">
+        <v>45301.809500000003</v>
+      </c>
+      <c r="K85" s="26">
+        <v>44823.281576000001</v>
       </c>
     </row>
   </sheetData>
@@ -2774,5 +3487,196 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37E36BC-E36C-432F-90D7-E660A09B53A5}">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="14">
+        <v>110022</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="15">
+        <v>40410</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="10">
+        <v>41180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="D9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="10">
+        <v>43005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="D10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="10">
+        <v>43061</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="D11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" s="10">
+        <v>43110</v>
+      </c>
+      <c r="H11" s="10">
+        <v>43647</v>
+      </c>
+      <c r="I11">
+        <v>2.9039999999999999</v>
+      </c>
+      <c r="J11" s="12">
+        <v>4.1200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="H12" s="10">
+        <v>43648</v>
+      </c>
+      <c r="I12">
+        <v>2.915</v>
+      </c>
+      <c r="J12" s="12">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="H13" s="10">
+        <v>43649</v>
+      </c>
+      <c r="I13">
+        <v>2.859</v>
+      </c>
+      <c r="J13" s="13">
+        <v>-1.9199999999999998E-2</v>
+      </c>
+      <c r="K13" s="11">
+        <f>SUM(J11:J15)</f>
+        <v>3.8599999999999995E-2</v>
+      </c>
+      <c r="L13" t="s">
+        <v>101</v>
+      </c>
+      <c r="M13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="H14" s="10">
+        <v>43650</v>
+      </c>
+      <c r="I14">
+        <v>2.8380000000000001</v>
+      </c>
+      <c r="J14" s="13">
+        <v>-7.3000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="H15" s="10">
+        <v>43651</v>
+      </c>
+      <c r="I15">
+        <v>2.895</v>
+      </c>
+      <c r="J15" s="12">
+        <v>2.01E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>